<commit_message>
changed excel test files
</commit_message>
<xml_diff>
--- a/test data/graph - Copy.xlsx
+++ b/test data/graph - Copy.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
color for the tabs
</commit_message>
<xml_diff>
--- a/test data/graph - Copy.xlsx
+++ b/test data/graph - Copy.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
I am going to cry soon
</commit_message>
<xml_diff>
--- a/test data/graph - Copy.xlsx
+++ b/test data/graph - Copy.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
fittings now can be save as
</commit_message>
<xml_diff>
--- a/test data/graph - Copy.xlsx
+++ b/test data/graph - Copy.xlsx
@@ -467,202 +467,202 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>-0.1152038588422199</v>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>35.77268174030434</v>
       </c>
       <c r="C2" t="n">
-        <v>49</v>
+        <v>71.66056733945092</v>
       </c>
       <c r="D2" t="n">
-        <v>73</v>
+        <v>107.5484529385974</v>
       </c>
       <c r="E2" t="n">
-        <v>97</v>
+        <v>143.436338537744</v>
       </c>
       <c r="F2" t="n">
-        <v>121</v>
+        <v>179.3242241368905</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>-0.4419583619815833</v>
       </c>
       <c r="B3" t="n">
-        <v>345</v>
+        <v>-593.5971618491448</v>
       </c>
       <c r="C3" t="n">
-        <v>688</v>
+        <v>-1186.752365336308</v>
       </c>
       <c r="D3" t="n">
-        <v>1031</v>
+        <v>-1779.907568823471</v>
       </c>
       <c r="E3" t="n">
-        <v>1374</v>
+        <v>-2373.062772310634</v>
       </c>
       <c r="F3" t="n">
-        <v>1717</v>
+        <v>-2966.217975797797</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>-0.5311650342112434</v>
       </c>
       <c r="B4" t="n">
-        <v>2345</v>
+        <v>1053.468908287305</v>
       </c>
       <c r="C4" t="n">
-        <v>4687</v>
+        <v>2107.468981608821</v>
       </c>
       <c r="D4" t="n">
-        <v>7029</v>
+        <v>3161.469054930337</v>
       </c>
       <c r="E4" t="n">
-        <v>9371</v>
+        <v>4215.469128251852</v>
       </c>
       <c r="F4" t="n">
-        <v>11713</v>
+        <v>5269.469201573368</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>-0.6203717064409036</v>
       </c>
       <c r="B5" t="n">
-        <v>66</v>
+        <v>-3360.906366221488</v>
       </c>
       <c r="C5" t="n">
-        <v>128</v>
+        <v>-6721.192360736537</v>
       </c>
       <c r="D5" t="n">
-        <v>190</v>
+        <v>-10081.47835525158</v>
       </c>
       <c r="E5" t="n">
-        <v>252</v>
+        <v>-13441.76434976663</v>
       </c>
       <c r="F5" t="n">
-        <v>314</v>
+        <v>-16802.05034428168</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>-0.7095783786705637</v>
       </c>
       <c r="B6" t="n">
-        <v>8568</v>
+        <v>3533.876217783167</v>
       </c>
       <c r="C6" t="n">
-        <v>17131</v>
+        <v>7068.462013945003</v>
       </c>
       <c r="D6" t="n">
-        <v>25694</v>
+        <v>10603.04781010684</v>
       </c>
       <c r="E6" t="n">
-        <v>34257</v>
+        <v>14137.63360626868</v>
       </c>
       <c r="F6" t="n">
-        <v>42820</v>
+        <v>17672.21940243051</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>-0.7987850509002239</v>
       </c>
       <c r="B7" t="n">
-        <v>78</v>
+        <v>-5269.43116454829</v>
       </c>
       <c r="C7" t="n">
-        <v>150</v>
+        <v>-10538.06354404568</v>
       </c>
       <c r="D7" t="n">
-        <v>222</v>
+        <v>-15806.69592354307</v>
       </c>
       <c r="E7" t="n">
-        <v>294</v>
+        <v>-21075.32830304046</v>
       </c>
       <c r="F7" t="n">
-        <v>366</v>
+        <v>-26343.96068253785</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>-0.8879917231298838</v>
       </c>
       <c r="B8" t="n">
-        <v>6578</v>
+        <v>4162.228615608765</v>
       </c>
       <c r="C8" t="n">
-        <v>13149</v>
+        <v>8325.345222940659</v>
       </c>
       <c r="D8" t="n">
-        <v>19720</v>
+        <v>12488.46183027255</v>
       </c>
       <c r="E8" t="n">
-        <v>26291</v>
+        <v>16651.57843760445</v>
       </c>
       <c r="F8" t="n">
-        <v>32862</v>
+        <v>20814.69504493634</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>-0.9771983953595438</v>
       </c>
       <c r="B9" t="n">
-        <v>676</v>
+        <v>-3790.527778620944</v>
       </c>
       <c r="C9" t="n">
-        <v>1344</v>
+        <v>-7580.078358846528</v>
       </c>
       <c r="D9" t="n">
-        <v>2012</v>
+        <v>-11369.62893907211</v>
       </c>
       <c r="E9" t="n">
-        <v>2680</v>
+        <v>-15159.1795192977</v>
       </c>
       <c r="F9" t="n">
-        <v>3348</v>
+        <v>-18948.73009952328</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>-1.677071072957392</v>
       </c>
       <c r="B10" t="n">
-        <v>5677</v>
+        <v>1608.419437684537</v>
       </c>
       <c r="C10" t="n">
-        <v>11345</v>
+        <v>3218.515946442029</v>
       </c>
       <c r="D10" t="n">
-        <v>17013</v>
+        <v>4828.612455199524</v>
       </c>
       <c r="E10" t="n">
-        <v>22681</v>
+        <v>6438.708963957018</v>
       </c>
       <c r="F10" t="n">
-        <v>28349</v>
+        <v>8048.805472714512</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>1.435940288367797</v>
       </c>
       <c r="B11" t="n">
-        <v>4893</v>
+        <v>-571.7594332423268</v>
       </c>
       <c r="C11" t="n">
-        <v>9776</v>
+        <v>-1144.954806773022</v>
       </c>
       <c r="D11" t="n">
-        <v>14659</v>
+        <v>-1718.150180303716</v>
       </c>
       <c r="E11" t="n">
-        <v>19542</v>
+        <v>-2291.345553834411</v>
       </c>
       <c r="F11" t="n">
-        <v>24425</v>
+        <v>-2864.540927365107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving works good for one fitting i ll do the rest
</commit_message>
<xml_diff>
--- a/test data/graph - Copy.xlsx
+++ b/test data/graph - Copy.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Original Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Fitted Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -668,4 +669,835 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y_poly_fit_deg_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-519.854545454552</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.090909090909091</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-354.6952667167593</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.181818181818182</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-194.2839218632639</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.272727272727273</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-38.5432506887073</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.363636363636364</v>
+      </c>
+      <c r="B6" t="n">
+        <v>112.6040070122713</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.454545454545455</v>
+      </c>
+      <c r="B7" t="n">
+        <v>259.2351114450298</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.545454545454545</v>
+      </c>
+      <c r="B8" t="n">
+        <v>401.4273228149277</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.636363636363636</v>
+      </c>
+      <c r="B9" t="n">
+        <v>539.2579013273253</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.727272727272727</v>
+      </c>
+      <c r="B10" t="n">
+        <v>672.8041071875823</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1.818181818181818</v>
+      </c>
+      <c r="B11" t="n">
+        <v>802.1432006010568</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.909090909090909</v>
+      </c>
+      <c r="B12" t="n">
+        <v>927.3524417731087</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1048.509090909098</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2.090909090909091</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1165.690408214382</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2.181818181818182</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1278.973653894323</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2.272727272727272</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1388.436088154278</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2.363636363636364</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1494.154971199609</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2.454545454545455</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1596.207563235673</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2.545454545454545</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1694.671124467829</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2.636363636363637</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1789.622915101439</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2.727272727272728</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1881.14019534186</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2.818181818181818</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1969.300225394452</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2.909090909090909</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2054.180265464574</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2135.857575757587</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>3.090909090909091</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2214.40941647885</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3.181818181818182</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2289.91304783372</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3.272727272727273</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2362.44573002756</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>3.363636363636364</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2432.084723265727</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3.454545454545455</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2498.90728775358</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3.545454545454545</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2562.99068369648</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3.636363636363636</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2624.412171299786</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>3.727272727272728</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2683.249010768857</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>3.818181818181818</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2739.578462309052</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3.909090909090909</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2793.477786125731</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2845.024242424253</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>4.090909090909091</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2894.295091409978</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>4.181818181818182</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2941.367593288265</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>4.272727272727273</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2986.319008264473</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>4.363636363636363</v>
+      </c>
+      <c r="B39" t="n">
+        <v>3029.226596543961</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>4.454545454545455</v>
+      </c>
+      <c r="B40" t="n">
+        <v>3070.167618332091</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>4.545454545454545</v>
+      </c>
+      <c r="B41" t="n">
+        <v>3109.219333834219</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>4.636363636363637</v>
+      </c>
+      <c r="B42" t="n">
+        <v>3146.459003255705</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>4.727272727272728</v>
+      </c>
+      <c r="B43" t="n">
+        <v>3181.963886801911</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>4.818181818181818</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3215.811244678194</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>4.909090909090909</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3248.078337089914</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>5</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3278.842424242431</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>5.090909090909091</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3308.180766341102</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>5.181818181818182</v>
+      </c>
+      <c r="B48" t="n">
+        <v>3336.170623591289</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>5.272727272727272</v>
+      </c>
+      <c r="B49" t="n">
+        <v>3362.889256198351</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>5.363636363636363</v>
+      </c>
+      <c r="B50" t="n">
+        <v>3388.413924367647</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>5.454545454545455</v>
+      </c>
+      <c r="B51" t="n">
+        <v>3412.821888304536</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>5.545454545454546</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3436.190408214378</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>5.636363636363637</v>
+      </c>
+      <c r="B53" t="n">
+        <v>3458.596744302531</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>5.727272727272728</v>
+      </c>
+      <c r="B54" t="n">
+        <v>3480.118156774356</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>5.818181818181818</v>
+      </c>
+      <c r="B55" t="n">
+        <v>3500.831905835212</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>5.909090909090909</v>
+      </c>
+      <c r="B56" t="n">
+        <v>3520.815251690458</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>6</v>
+      </c>
+      <c r="B57" t="n">
+        <v>3540.145454545453</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>6.090909090909091</v>
+      </c>
+      <c r="B58" t="n">
+        <v>3558.899774605557</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>6.181818181818182</v>
+      </c>
+      <c r="B59" t="n">
+        <v>3577.155472076131</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>6.272727272727272</v>
+      </c>
+      <c r="B60" t="n">
+        <v>3594.989807162531</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>6.363636363636364</v>
+      </c>
+      <c r="B61" t="n">
+        <v>3612.48004007012</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>6.454545454545455</v>
+      </c>
+      <c r="B62" t="n">
+        <v>3629.703431004252</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>6.545454545454546</v>
+      </c>
+      <c r="B63" t="n">
+        <v>3646.737240170293</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>6.636363636363637</v>
+      </c>
+      <c r="B64" t="n">
+        <v>3663.658727773599</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>6.727272727272728</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3680.545154019528</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>6.818181818181818</v>
+      </c>
+      <c r="B66" t="n">
+        <v>3697.473779113441</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>6.909090909090909</v>
+      </c>
+      <c r="B67" t="n">
+        <v>3714.521863260698</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>7</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3731.766666666658</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>7.090909090909091</v>
+      </c>
+      <c r="B69" t="n">
+        <v>3749.28544953668</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>7.181818181818182</v>
+      </c>
+      <c r="B70" t="n">
+        <v>3767.155472076123</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>7.272727272727272</v>
+      </c>
+      <c r="B71" t="n">
+        <v>3785.453994490346</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>7.363636363636364</v>
+      </c>
+      <c r="B72" t="n">
+        <v>3804.258276984711</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>7.454545454545455</v>
+      </c>
+      <c r="B73" t="n">
+        <v>3823.645579764576</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>7.545454545454546</v>
+      </c>
+      <c r="B74" t="n">
+        <v>3843.693163035299</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>7.636363636363637</v>
+      </c>
+      <c r="B75" t="n">
+        <v>3864.478287002241</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>7.727272727272728</v>
+      </c>
+      <c r="B76" t="n">
+        <v>3886.078211870762</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>7.818181818181818</v>
+      </c>
+      <c r="B77" t="n">
+        <v>3908.570197846217</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>7.909090909090909</v>
+      </c>
+      <c r="B78" t="n">
+        <v>3932.031505133969</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>8</v>
+      </c>
+      <c r="B79" t="n">
+        <v>3956.539393939379</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>8.09090909090909</v>
+      </c>
+      <c r="B80" t="n">
+        <v>3982.171124467804</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>8.181818181818182</v>
+      </c>
+      <c r="B81" t="n">
+        <v>4009.003956924602</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>8.272727272727273</v>
+      </c>
+      <c r="B82" t="n">
+        <v>4037.115151515136</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>8.363636363636363</v>
+      </c>
+      <c r="B83" t="n">
+        <v>4066.581968444762</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>8.454545454545455</v>
+      </c>
+      <c r="B84" t="n">
+        <v>4097.48166791884</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>8.545454545454547</v>
+      </c>
+      <c r="B85" t="n">
+        <v>4129.891510142735</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>8.636363636363637</v>
+      </c>
+      <c r="B86" t="n">
+        <v>4163.888755321795</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>8.727272727272727</v>
+      </c>
+      <c r="B87" t="n">
+        <v>4199.55066366139</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>8.818181818181818</v>
+      </c>
+      <c r="B88" t="n">
+        <v>4236.954495366876</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>8.90909090909091</v>
+      </c>
+      <c r="B89" t="n">
+        <v>4276.177510643608</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>9</v>
+      </c>
+      <c r="B90" t="n">
+        <v>4317.296969696951</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>9.090909090909092</v>
+      </c>
+      <c r="B91" t="n">
+        <v>4360.390132732266</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>9.181818181818182</v>
+      </c>
+      <c r="B92" t="n">
+        <v>4405.534259954902</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>9.272727272727273</v>
+      </c>
+      <c r="B93" t="n">
+        <v>4452.80661157023</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>9.363636363636363</v>
+      </c>
+      <c r="B94" t="n">
+        <v>4502.284447783604</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>9.454545454545455</v>
+      </c>
+      <c r="B95" t="n">
+        <v>4554.045028800382</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>9.545454545454545</v>
+      </c>
+      <c r="B96" t="n">
+        <v>4608.165614825929</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>9.636363636363637</v>
+      </c>
+      <c r="B97" t="n">
+        <v>4664.723466065597</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>9.727272727272727</v>
+      </c>
+      <c r="B98" t="n">
+        <v>4723.79584272475</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>9.818181818181818</v>
+      </c>
+      <c r="B99" t="n">
+        <v>4785.46000500875</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>9.90909090909091</v>
+      </c>
+      <c r="B100" t="n">
+        <v>4849.793213122949</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>10</v>
+      </c>
+      <c r="B101" t="n">
+        <v>4916.872727272713</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>